<commit_message>
Excel database updates for capturing API weather data
</commit_message>
<xml_diff>
--- a/OmnisharpDatabase01.xlsx
+++ b/OmnisharpDatabase01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carston\Documents\Omnisharp\Project - Map\OmniLocations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carston\Documents\Omnisharp\Project - Fluffy Map\OmniMap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1000B865-A727-4BE9-B5AF-A2710108A38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B75066-57EC-4A0D-A221-1BF9DB6DC751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C10BDBA5-96E2-4E11-9AC1-ECA6267D2D2B}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="106">
   <si>
     <t>Amarillo</t>
   </si>
@@ -385,6 +385,12 @@
   </si>
   <si>
     <t>Olathe, KS</t>
+  </si>
+  <si>
+    <t>TodayHigh</t>
+  </si>
+  <si>
+    <t>TodayLow</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -482,6 +488,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -817,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26851CE-C6E3-471D-B829-4B0087AEFA41}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,9 +844,11 @@
     <col min="17" max="17" width="14.5703125" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" style="6" customWidth="1"/>
     <col min="19" max="19" width="68" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -900,8 +909,14 @@
       <c r="T1" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -936,7 +951,7 @@
         <v>79108</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -968,7 +983,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1003,7 +1018,7 @@
         <v>68776</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>67851</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1082,7 +1097,7 @@
         <v>54303</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1117,7 +1132,7 @@
         <v>61257</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1146,7 +1161,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1181,7 +1196,7 @@
         <v>28850</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1216,7 +1231,7 @@
         <v>68107</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1254,7 +1269,7 @@
         <v>99360</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1289,7 +1304,7 @@
         <v>49080</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1318,7 +1333,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1353,7 +1368,7 @@
         <v>28392</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1388,7 +1403,7 @@
         <v>19446</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Travel and New Plant updates
</commit_message>
<xml_diff>
--- a/OmnisharpDatabase01.xlsx
+++ b/OmnisharpDatabase01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carston\Documents\Omnisharp\Project - Fluffy Map\OmniMap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B75066-57EC-4A0D-A221-1BF9DB6DC751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5E6B9A-531F-444C-9CCC-10A92B41D075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C10BDBA5-96E2-4E11-9AC1-ECA6267D2D2B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C10BDBA5-96E2-4E11-9AC1-ECA6267D2D2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="111">
   <si>
     <t>Amarillo</t>
   </si>
@@ -391,6 +391,21 @@
   </si>
   <si>
     <t>TodayLow</t>
+  </si>
+  <si>
+    <t>Grand Island</t>
+  </si>
+  <si>
+    <t>555 South Stuhr Road, Grand Island, NE 68801</t>
+  </si>
+  <si>
+    <t>Willmar</t>
+  </si>
+  <si>
+    <t>Jennie-O</t>
+  </si>
+  <si>
+    <t>2505 Willmar Ave SW, Willmar, MN 56201</t>
   </si>
 </sst>
 </file>
@@ -471,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -488,7 +503,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -824,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26851CE-C6E3-471D-B829-4B0087AEFA41}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,10 +923,10 @@
       <c r="T1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1064,7 +1078,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
         <v>58</v>
@@ -1072,9 +1086,6 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
@@ -1084,31 +1095,25 @@
       <c r="G6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L6" t="s">
-        <v>51</v>
-      </c>
       <c r="S6" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="T6">
-        <v>54303</v>
+        <v>68801</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
@@ -1120,97 +1125,97 @@
         <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="L7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T7">
-        <v>61257</v>
+        <v>54303</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>92</v>
+      </c>
+      <c r="L8" t="s">
+        <v>50</v>
       </c>
       <c r="S8" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="T8">
+        <v>61257</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>94</v>
-      </c>
-      <c r="L9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="S9" t="s">
-        <v>68</v>
-      </c>
-      <c r="T9">
-        <v>28850</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
         <v>31</v>
@@ -1219,30 +1224,30 @@
         <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T10">
-        <v>68107</v>
+        <v>28850</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -1257,33 +1262,30 @@
         <v>92</v>
       </c>
       <c r="L11" t="s">
-        <v>52</v>
-      </c>
-      <c r="R11" s="6">
-        <v>45691</v>
+        <v>51</v>
       </c>
       <c r="S11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T11">
-        <v>99360</v>
+        <v>68107</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
         <v>31</v>
@@ -1292,59 +1294,68 @@
         <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L12" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="R12" s="6">
+        <v>45691</v>
       </c>
       <c r="S12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T12">
-        <v>49080</v>
+        <v>99360</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
         <v>27</v>
       </c>
       <c r="H13" t="s">
-        <v>91</v>
+        <v>94</v>
+      </c>
+      <c r="L13" t="s">
+        <v>51</v>
       </c>
       <c r="S13" t="s">
-        <v>81</v>
+        <v>71</v>
+      </c>
+      <c r="T13">
+        <v>49080</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
@@ -1356,24 +1367,18 @@
         <v>27</v>
       </c>
       <c r="H14" t="s">
-        <v>92</v>
-      </c>
-      <c r="L14" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="S14" t="s">
-        <v>72</v>
-      </c>
-      <c r="T14">
-        <v>28392</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1382,141 +1387,147 @@
         <v>21</v>
       </c>
       <c r="E15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L15" t="s">
         <v>51</v>
       </c>
       <c r="S15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T15">
-        <v>19446</v>
+        <v>28392</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="E16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>92</v>
-      </c>
-      <c r="J16" t="s">
-        <v>43</v>
+        <v>93</v>
+      </c>
+      <c r="L16" t="s">
+        <v>51</v>
       </c>
       <c r="S16" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="T16">
-        <v>72761</v>
+        <v>19446</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="E17" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H17" t="s">
         <v>92</v>
       </c>
-      <c r="L17" t="s">
-        <v>52</v>
+      <c r="J17" t="s">
+        <v>43</v>
       </c>
       <c r="S17" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="T17">
-        <v>50588</v>
+        <v>72761</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G18" t="s">
         <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>53</v>
+        <v>92</v>
+      </c>
+      <c r="L18" t="s">
+        <v>52</v>
       </c>
       <c r="S18" t="s">
-        <v>82</v>
+        <v>74</v>
+      </c>
+      <c r="T18">
+        <v>50588</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E19" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>31</v>
@@ -1525,85 +1536,76 @@
         <v>27</v>
       </c>
       <c r="H19" t="s">
-        <v>94</v>
-      </c>
-      <c r="L19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="S19" t="s">
-        <v>75</v>
-      </c>
-      <c r="T19">
-        <v>85353</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
       <c r="E20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>94</v>
       </c>
       <c r="L20" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="S20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T20">
-        <v>78664</v>
+        <v>85353</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="D21" t="s">
-        <v>51</v>
-      </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G21" t="s">
-        <v>85</v>
-      </c>
-      <c r="J21" t="s">
-        <v>98</v>
-      </c>
-      <c r="K21" t="s">
-        <v>97</v>
-      </c>
-      <c r="L21" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="S21" t="s">
-        <v>99</v>
+        <v>110</v>
+      </c>
+      <c r="T21">
+        <v>56201</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
         <v>59</v>
@@ -1611,23 +1613,23 @@
       <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="D22" t="s">
-        <v>52</v>
-      </c>
       <c r="E22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L22" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="S22" t="s">
-        <v>103</v>
+        <v>76</v>
+      </c>
+      <c r="T22">
+        <v>78664</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -1641,7 +1643,7 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="E23" s="2">
         <v>0</v>
@@ -1652,16 +1654,22 @@
       <c r="G23" t="s">
         <v>85</v>
       </c>
+      <c r="J23" t="s">
+        <v>98</v>
+      </c>
+      <c r="K23" t="s">
+        <v>97</v>
+      </c>
       <c r="L23" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="S23" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
         <v>59</v>
@@ -1670,7 +1678,7 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
@@ -1681,22 +1689,16 @@
       <c r="G24" t="s">
         <v>85</v>
       </c>
-      <c r="K24" t="s">
-        <v>95</v>
-      </c>
       <c r="L24" t="s">
-        <v>86</v>
-      </c>
-      <c r="S24" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="T24">
-        <v>66617</v>
+        <v>52</v>
+      </c>
+      <c r="S24" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
         <v>59</v>
@@ -1705,24 +1707,88 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" t="s">
+        <v>85</v>
+      </c>
+      <c r="L25" t="s">
+        <v>89</v>
+      </c>
+      <c r="S25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" t="s">
+        <v>85</v>
+      </c>
+      <c r="K26" t="s">
+        <v>95</v>
+      </c>
+      <c r="L26" t="s">
+        <v>86</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="T26">
+        <v>66617</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>88</v>
       </c>
-      <c r="G25" t="s">
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
         <v>88</v>
       </c>
-      <c r="K25" t="s">
+      <c r="G27" t="s">
+        <v>88</v>
+      </c>
+      <c r="K27" t="s">
         <v>96</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L27" t="s">
         <v>90</v>
       </c>
-      <c r="S25" t="s">
+      <c r="S27" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added JennieO and Greater Omaha
</commit_message>
<xml_diff>
--- a/OmnisharpDatabase01.xlsx
+++ b/OmnisharpDatabase01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carston\Documents\Omnisharp\Project - Fluffy Map\OmniMap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5E6B9A-531F-444C-9CCC-10A92B41D075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364620FB-551F-4140-A266-23D5FA52C42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C10BDBA5-96E2-4E11-9AC1-ECA6267D2D2B}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="113">
   <si>
     <t>Amarillo</t>
   </si>
@@ -406,13 +406,19 @@
   </si>
   <si>
     <t>2505 Willmar Ave SW, Willmar, MN 56201</t>
+  </si>
+  <si>
+    <t>Greater Omaha</t>
+  </si>
+  <si>
+    <t>3001 L St, Omaha, NE 68107</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,12 +455,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -486,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -502,7 +502,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -838,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26851CE-C6E3-471D-B829-4B0087AEFA41}">
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,16 +1103,10 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
@@ -1124,31 +1117,28 @@
       <c r="G7" t="s">
         <v>27</v>
       </c>
-      <c r="H7" t="s">
-        <v>53</v>
-      </c>
       <c r="L7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S7" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="T7">
-        <v>54303</v>
+        <v>68107</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
@@ -1160,50 +1150,44 @@
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T8">
-        <v>61257</v>
+        <v>54303</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="H9" t="s">
-        <v>53</v>
-      </c>
       <c r="S9" t="s">
-        <v>80</v>
+        <v>110</v>
+      </c>
+      <c r="T9">
+        <v>56201</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
@@ -1212,10 +1196,10 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>31</v>
@@ -1224,56 +1208,50 @@
         <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L10" t="s">
         <v>50</v>
       </c>
       <c r="S10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T10">
-        <v>28850</v>
+        <v>61257</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
         <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="S11" t="s">
-        <v>69</v>
-      </c>
-      <c r="T11">
-        <v>68107</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>57</v>
@@ -1282,10 +1260,10 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>31</v>
@@ -1294,24 +1272,21 @@
         <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L12" t="s">
-        <v>52</v>
-      </c>
-      <c r="R12" s="6">
-        <v>45691</v>
+        <v>50</v>
       </c>
       <c r="S12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="T12">
-        <v>99360</v>
+        <v>28850</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>58</v>
@@ -1323,7 +1298,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
         <v>31</v>
@@ -1332,260 +1307,272 @@
         <v>27</v>
       </c>
       <c r="H13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L13" t="s">
         <v>51</v>
       </c>
       <c r="S13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="T13">
-        <v>49080</v>
+        <v>68107</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
         <v>27</v>
       </c>
       <c r="H14" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="L14" t="s">
+        <v>52</v>
+      </c>
+      <c r="R14" s="6">
+        <v>45691</v>
       </c>
       <c r="S14" t="s">
-        <v>81</v>
+        <v>70</v>
+      </c>
+      <c r="T14">
+        <v>99360</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L15" t="s">
         <v>51</v>
       </c>
       <c r="S15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T15">
-        <v>28392</v>
+        <v>49080</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
         <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>93</v>
-      </c>
-      <c r="L16" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="S16" t="s">
-        <v>73</v>
-      </c>
-      <c r="T16">
-        <v>19446</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="E17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H17" t="s">
         <v>92</v>
       </c>
-      <c r="J17" t="s">
-        <v>43</v>
+      <c r="L17" t="s">
+        <v>51</v>
       </c>
       <c r="S17" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="T17">
-        <v>72761</v>
+        <v>28392</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
         <v>27</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T18">
-        <v>50588</v>
+        <v>19446</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="E19" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>92</v>
+      </c>
+      <c r="J19" t="s">
+        <v>43</v>
       </c>
       <c r="S19" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="T19">
+        <v>72761</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E20" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G20" t="s">
         <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="S20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T20">
-        <v>85353</v>
+        <v>50588</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
       </c>
       <c r="E21" s="2">
         <v>1</v>
@@ -1596,80 +1583,77 @@
       <c r="G21" t="s">
         <v>27</v>
       </c>
+      <c r="H21" t="s">
+        <v>53</v>
+      </c>
       <c r="S21" t="s">
-        <v>110</v>
-      </c>
-      <c r="T21">
-        <v>56201</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
       </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
       <c r="E22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>83</v>
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
+        <v>94</v>
       </c>
       <c r="L22" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="S22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T22">
-        <v>78664</v>
+        <v>85353</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
       </c>
-      <c r="D23" t="s">
-        <v>51</v>
-      </c>
       <c r="E23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>85</v>
-      </c>
-      <c r="J23" t="s">
-        <v>98</v>
-      </c>
-      <c r="K23" t="s">
-        <v>97</v>
-      </c>
-      <c r="L23" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="S23" t="s">
-        <v>99</v>
+        <v>110</v>
+      </c>
+      <c r="T23">
+        <v>56201</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
         <v>59</v>
@@ -1677,23 +1661,23 @@
       <c r="C24" t="s">
         <v>16</v>
       </c>
-      <c r="D24" t="s">
-        <v>52</v>
-      </c>
       <c r="E24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L24" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="S24" t="s">
-        <v>103</v>
+        <v>76</v>
+      </c>
+      <c r="T24">
+        <v>78664</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -1707,7 +1691,7 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
@@ -1718,16 +1702,22 @@
       <c r="G25" t="s">
         <v>85</v>
       </c>
+      <c r="J25" t="s">
+        <v>98</v>
+      </c>
+      <c r="K25" t="s">
+        <v>97</v>
+      </c>
       <c r="L25" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="S25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
@@ -1736,7 +1726,7 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
@@ -1747,22 +1737,16 @@
       <c r="G26" t="s">
         <v>85</v>
       </c>
-      <c r="K26" t="s">
-        <v>95</v>
-      </c>
       <c r="L26" t="s">
-        <v>86</v>
-      </c>
-      <c r="S26" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="T26">
-        <v>66617</v>
+        <v>52</v>
+      </c>
+      <c r="S26" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
@@ -1771,24 +1755,88 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
       </c>
       <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L27" t="s">
+        <v>89</v>
+      </c>
+      <c r="S27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" t="s">
+        <v>85</v>
+      </c>
+      <c r="K28" t="s">
+        <v>95</v>
+      </c>
+      <c r="L28" t="s">
+        <v>86</v>
+      </c>
+      <c r="S28" t="s">
+        <v>101</v>
+      </c>
+      <c r="T28">
+        <v>66617</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>88</v>
       </c>
-      <c r="G27" t="s">
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
         <v>88</v>
       </c>
-      <c r="K27" t="s">
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+      <c r="K29" t="s">
         <v>96</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L29" t="s">
         <v>90</v>
       </c>
-      <c r="S27" t="s">
+      <c r="S29" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>